<commit_message>
styled student page,added ece
</commit_message>
<xml_diff>
--- a/Student Data/ThirdYearStudents.xlsx
+++ b/Student Data/ThirdYearStudents.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Exam-Seat-Arrangement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Exam-Seat-Arrangement\Student Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77C2B1C-A891-45BC-8801-8C2071A5A023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3156CCE3-0883-479A-9120-E5EFADDA4E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csa" sheetId="1" r:id="rId1"/>
     <sheet name="csb" sheetId="2" r:id="rId2"/>
     <sheet name="eee" sheetId="3" r:id="rId3"/>
+    <sheet name="ece" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="217">
   <si>
     <t>rollnum</t>
   </si>
@@ -519,13 +520,172 @@
   </si>
   <si>
     <t>VISHNU M P</t>
+  </si>
+  <si>
+    <t>AAKASH MURALIDHARAN</t>
+  </si>
+  <si>
+    <t>ABHIJEET V</t>
+  </si>
+  <si>
+    <t>AISWARYA P K</t>
+  </si>
+  <si>
+    <t>AJU ANTONY</t>
+  </si>
+  <si>
+    <t>AKHILA K P</t>
+  </si>
+  <si>
+    <t>ALAN ALAPPATT</t>
+  </si>
+  <si>
+    <t>ALAN TOMY</t>
+  </si>
+  <si>
+    <t>ALEENA PAUL</t>
+  </si>
+  <si>
+    <t>ANDRIYA ANTO EMMATTY</t>
+  </si>
+  <si>
+    <t>ANEENA C BINU</t>
+  </si>
+  <si>
+    <t>ANUPAMA J</t>
+  </si>
+  <si>
+    <t>ASHWIN K P</t>
+  </si>
+  <si>
+    <t>ASWIN KRISHNA K S</t>
+  </si>
+  <si>
+    <t>ATHIRA FRANCIS</t>
+  </si>
+  <si>
+    <t>BHAVANA NARAYANAN</t>
+  </si>
+  <si>
+    <t>GAYATHRI R V</t>
+  </si>
+  <si>
+    <t>GOPIKA U</t>
+  </si>
+  <si>
+    <t>HENNA ROSE C S</t>
+  </si>
+  <si>
+    <t>JAYITHA HARIGOVIND</t>
+  </si>
+  <si>
+    <t>JIBIN SEBI</t>
+  </si>
+  <si>
+    <t>JINCY SUSAN JOHN</t>
+  </si>
+  <si>
+    <t>KAVYASREE A NAIR</t>
+  </si>
+  <si>
+    <t>KRISHNA K</t>
+  </si>
+  <si>
+    <t>M P ASWIN</t>
+  </si>
+  <si>
+    <t>MARIA VARGHESE</t>
+  </si>
+  <si>
+    <t>MUHAMMAD RASEEL</t>
+  </si>
+  <si>
+    <t>NANDANA VINOD</t>
+  </si>
+  <si>
+    <t>NAVIN T W</t>
+  </si>
+  <si>
+    <t>NOOPURA MOHAN</t>
+  </si>
+  <si>
+    <t>PARVATHY T R</t>
+  </si>
+  <si>
+    <t>RESHMA HENDRY</t>
+  </si>
+  <si>
+    <t>RESHMA ROY</t>
+  </si>
+  <si>
+    <t>SACHIN MANOHARAN</t>
+  </si>
+  <si>
+    <t>SANIL JOSEPH</t>
+  </si>
+  <si>
+    <t>SHIYAS S</t>
+  </si>
+  <si>
+    <t>SOWMYA M</t>
+  </si>
+  <si>
+    <t>STEEV VARGHESE U KOLLANNUR</t>
+  </si>
+  <si>
+    <t>TINIT THOMAS</t>
+  </si>
+  <si>
+    <t>UNNIMAYA SAJAYAN</t>
+  </si>
+  <si>
+    <t>VISAKH N R</t>
+  </si>
+  <si>
+    <t>ABHIJITH C S</t>
+  </si>
+  <si>
+    <t>ASHA S</t>
+  </si>
+  <si>
+    <t>ATHUL P S</t>
+  </si>
+  <si>
+    <t>JOSMAL MATHEW</t>
+  </si>
+  <si>
+    <t>MRIDULA J NAIR</t>
+  </si>
+  <si>
+    <t>NAVAKRISHNAN M R</t>
+  </si>
+  <si>
+    <t>NITHIN C T</t>
+  </si>
+  <si>
+    <t>SILPA SOMAN</t>
+  </si>
+  <si>
+    <t>SISIRA K M</t>
+  </si>
+  <si>
+    <t>SREEDEV J</t>
+  </si>
+  <si>
+    <t>SREEJITH V</t>
+  </si>
+  <si>
+    <t>VISHNU C</t>
+  </si>
+  <si>
+    <t>VIVEK NAIR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,13 +704,25 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -581,17 +753,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,7 +1058,7 @@
   <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,7 +2096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1212BC1A-6F2C-41B5-90C5-2A77E745D6D8}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1933,318 +2115,773 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>12013001</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>12013002</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>12013003</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>12013004</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>12013005</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>12013006</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>12013008</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>12013007</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>12013009</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>12013010</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>12013011</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12013022</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>12013012</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>12013014</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>12013015</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>12013016</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>12013017</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>12013018</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>12013019</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>12013020</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>12013021</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>12123024</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>12123025</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>12123026</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>12123027</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>12123028</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>12123029</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>12123030</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>12123031</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>12123032</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>12123033</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>12123034</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>12123035</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+      <c r="A35" s="2">
         <v>12123036</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+      <c r="A36" s="2">
         <v>12123038</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>12123039</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+      <c r="A38" s="2">
         <v>12123040</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+      <c r="A39" s="2">
         <v>12123041</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
+      <c r="A40" s="2">
         <v>12123042</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>163</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE94710-5F55-4209-991F-C60DF91A7375}">
+  <dimension ref="A1:B55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>12014001</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>12014002</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>12014003</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>12014004</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>12014005</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>12014006</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>12014007</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>12014008</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>12014009</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>12014010</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>12014011</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12014012</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>12014013</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>12014014</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>12014015</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>12014016</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>12014017</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>12014018</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>12014019</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>12014020</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>12014021</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>12014022</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>12014023</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>12014024</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>12014025</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>12014026</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>12014027</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>12014028</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>12014029</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>12014030</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>12014031</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>12014032</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>12014033</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>12014035</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>12014037</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>12014038</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>12014039</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>12014040</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>12014041</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>12014042</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>12124043</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>12124044</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>12124045</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>12124046</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>12124047</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>12124048</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>12124049</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>12124050</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>12124051</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>12124052</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>12124053</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>12124054</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>12124055</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>